<commit_message>
working new line chart into flaskapp and updating data with new category labels
</commit_message>
<xml_diff>
--- a/Final_Data/CPI_Category_Tree_Final - REVISED.xlsx
+++ b/Final_Data/CPI_Category_Tree_Final - REVISED.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salinger\Documents\MIDS\W209\final project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamst\Documents\Viz\W209-Final\Final_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A3F6E3-E383-4103-87AD-9A3049FC05B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DF6732-8EB9-4A64-BE2A-A2D515E49869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1CCC2A7C-B94B-48C8-B4F9-530ABEF37C54}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CCC2A7C-B94B-48C8-B4F9-530ABEF37C54}"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="559">
   <si>
     <t>Series ID</t>
   </si>
@@ -1491,6 +1491,231 @@
   </si>
   <si>
     <t>Revised Name with CPI</t>
+  </si>
+  <si>
+    <t>CPI - Food &amp; Beverages</t>
+  </si>
+  <si>
+    <t>CPI - Cereals &amp; bakery products</t>
+  </si>
+  <si>
+    <t>CPI - Meats, poultry, fish, &amp; eggs</t>
+  </si>
+  <si>
+    <t>CPI - Dairy &amp; related goods</t>
+  </si>
+  <si>
+    <t>CPI - Fruits &amp; vegetables</t>
+  </si>
+  <si>
+    <t>CPI - Meals &amp; snacks (full-service)</t>
+  </si>
+  <si>
+    <t>CPI - Food at work &amp; schools</t>
+  </si>
+  <si>
+    <t>CPI - Beer &amp; related drinks at home</t>
+  </si>
+  <si>
+    <t>CPI - Alcoholic beverages (away)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPI - Nonalcoholic beverages </t>
+  </si>
+  <si>
+    <t>CPI - Nonfrozen noncarbonated drinks</t>
+  </si>
+  <si>
+    <t>CPI - Other beverages (e.g. tea)</t>
+  </si>
+  <si>
+    <t>CPI - Lodging away from goods</t>
+  </si>
+  <si>
+    <t>CPI - Owners' equivalent rent</t>
+  </si>
+  <si>
+    <t>CPI - Fuels &amp; utilities</t>
+  </si>
+  <si>
+    <t>CPI - Fuel oil &amp; other fuels</t>
+  </si>
+  <si>
+    <t>CPI - Water &amp; sewerage maint.</t>
+  </si>
+  <si>
+    <t>CPI - Garbage &amp; trash collection</t>
+  </si>
+  <si>
+    <t>CPI - HH furnishings &amp; operations</t>
+  </si>
+  <si>
+    <t>CPI - Window &amp; floor coverings</t>
+  </si>
+  <si>
+    <t>CPI - Furniture &amp; bedding</t>
+  </si>
+  <si>
+    <t>CPI - Tools &amp; outdoor equipment</t>
+  </si>
+  <si>
+    <t>CPI - Other HH equipment &amp; furnishing</t>
+  </si>
+  <si>
+    <t>CPI - Men's suits &amp; outerwear</t>
+  </si>
+  <si>
+    <t>CPI - Men's underwear, pajama &amp; swim</t>
+  </si>
+  <si>
+    <t>CPI - Men's shirts &amp; sweaters</t>
+  </si>
+  <si>
+    <t>CPI - Men's pants &amp; shorts</t>
+  </si>
+  <si>
+    <t>CPI - Women's &amp; girls' goods</t>
+  </si>
+  <si>
+    <t>CPI - Women's suits &amp; separates</t>
+  </si>
+  <si>
+    <t>CPI - Women's underwear, pajama &amp; swim</t>
+  </si>
+  <si>
+    <t>CPI - Boys' &amp; girls' footwear</t>
+  </si>
+  <si>
+    <t>CPI - Infants' &amp; toddlers' apparel</t>
+  </si>
+  <si>
+    <t>CPI - Jewelry &amp; watches</t>
+  </si>
+  <si>
+    <t>CPI - Used cars &amp; trucks</t>
+  </si>
+  <si>
+    <t>CPI - Leased cars &amp; trucks</t>
+  </si>
+  <si>
+    <t>CPI - Motor vehicle parts &amp; equipment</t>
+  </si>
+  <si>
+    <t>CPI - Motor vehicle maint. &amp; repair</t>
+  </si>
+  <si>
+    <t>CPI - Eyeglasses &amp; eye care</t>
+  </si>
+  <si>
+    <t>CPI - Nursing homes &amp; day services</t>
+  </si>
+  <si>
+    <t>CPI - Video &amp; audio</t>
+  </si>
+  <si>
+    <t>CPI - Cable &amp; satellite TV service</t>
+  </si>
+  <si>
+    <t>CPI - Pets, pet products &amp; services</t>
+  </si>
+  <si>
+    <t>CPI - Pets &amp; pet products</t>
+  </si>
+  <si>
+    <t>CPI - Pet services (e.g. veterinary)</t>
+  </si>
+  <si>
+    <t>CPI - Sports vehicles like bicycles</t>
+  </si>
+  <si>
+    <t>CPI - Photo equipment &amp; supplies</t>
+  </si>
+  <si>
+    <t>CPI - Sewing machines, fabric &amp; supplies</t>
+  </si>
+  <si>
+    <t>CPI - Music instruments &amp; accessories</t>
+  </si>
+  <si>
+    <t>CPI - Other recreational services</t>
+  </si>
+  <si>
+    <t>CPI - Club membership</t>
+  </si>
+  <si>
+    <t>CPI - Education &amp; communication</t>
+  </si>
+  <si>
+    <t>CPI - Educational books &amp; supplies</t>
+  </si>
+  <si>
+    <t>CPI - College tuition &amp; fees</t>
+  </si>
+  <si>
+    <t>CPI - Elementary &amp; H.S. tuition and fees</t>
+  </si>
+  <si>
+    <t>CPI - Day care &amp; preschool</t>
+  </si>
+  <si>
+    <t>CPI - Tech. and businses school costs</t>
+  </si>
+  <si>
+    <t>CPI - Postage &amp; delivery services</t>
+  </si>
+  <si>
+    <t>CPI - Computers &amp; peripherals</t>
+  </si>
+  <si>
+    <t>CPI - Internet services &amp; elec. providers</t>
+  </si>
+  <si>
+    <t>CPI - Tobacco &amp; smoking products</t>
+  </si>
+  <si>
+    <t>CPI - Misc. personal services</t>
+  </si>
+  <si>
+    <t>CPI - Laundry &amp; dry cleaning services</t>
+  </si>
+  <si>
+    <t>CPI* - Meals &amp; snacks (limited)</t>
+  </si>
+  <si>
+    <t>CPI* - Food from vendors &amp; machines</t>
+  </si>
+  <si>
+    <t>CPI* - Frozen noncarbonated drinks</t>
+  </si>
+  <si>
+    <t>CPI* - Tenants' &amp; household insurance</t>
+  </si>
+  <si>
+    <t>CPI* - Medical equipment &amp; supplies</t>
+  </si>
+  <si>
+    <t>CPI* - Video discs &amp; other (e.g. rental)</t>
+  </si>
+  <si>
+    <t>CPI* - Recorded music &amp; subscriptions</t>
+  </si>
+  <si>
+    <t>CPI* - Photographers &amp; photo processing</t>
+  </si>
+  <si>
+    <t>CPI* - Newspapers &amp; magazines</t>
+  </si>
+  <si>
+    <t>CPI* - Info. &amp; info. Processing</t>
+  </si>
+  <si>
+    <t>CPI* - Computer software &amp; accessories</t>
+  </si>
+  <si>
+    <t>CPI* - Non-cigarette tabacco products</t>
+  </si>
+  <si>
+    <t>CPI* - Other apparel services</t>
   </si>
 </sst>
 </file>
@@ -1854,19 +2079,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB36D4E-21E8-4B44-992A-C0473451182F}">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="80.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="80.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="80.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1889,16 +2116,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>200</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f>_xlfn.CONCAT("CPI - ",B2)</f>
-        <v>CPI - All items</v>
+      <c r="C2" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -1913,16 +2139,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>201</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f t="shared" ref="C3:C66" si="0">_xlfn.CONCAT("CPI - ",B3)</f>
-        <v>CPI - Food &amp; Beverages</v>
+      <c r="C3" s="1" t="s">
+        <v>484</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
@@ -1937,16 +2162,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Food at home</v>
+      <c r="C4" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -1961,16 +2185,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="C5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Cereals &amp; bakery products</v>
+      <c r="C5" s="1" t="s">
+        <v>485</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
@@ -1985,16 +2208,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Meats, poultry, fish, &amp; eggs</v>
+      <c r="C6" s="1" t="s">
+        <v>486</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
@@ -2009,16 +2231,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>205</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Dairy &amp; related goods</v>
+      <c r="C7" s="1" t="s">
+        <v>487</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -2033,16 +2254,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>206</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Fruits &amp; vegetables</v>
+      <c r="C8" s="1" t="s">
+        <v>488</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
@@ -2057,16 +2277,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="C9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Other food at home</v>
+      <c r="C9" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>
@@ -2081,16 +2300,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="C10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Food away from home</v>
+      <c r="C10" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="D10" t="s">
         <v>37</v>
@@ -2105,16 +2323,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Meals &amp; snacks (full-service)</v>
+      <c r="C11" s="1" t="s">
+        <v>489</v>
       </c>
       <c r="D11" t="s">
         <v>38</v>
@@ -2129,16 +2346,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="C12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Meals &amp; snacks (limited)</v>
+      <c r="C12" s="1" t="s">
+        <v>546</v>
       </c>
       <c r="D12" t="s">
         <v>177</v>
@@ -2153,16 +2369,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>211</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Food at work &amp; schools</v>
+      <c r="C13" s="1" t="s">
+        <v>490</v>
       </c>
       <c r="D13" t="s">
         <v>40</v>
@@ -2177,16 +2392,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="C14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Food from vendors &amp; machines</v>
+      <c r="C14" s="1" t="s">
+        <v>547</v>
       </c>
       <c r="D14" t="s">
         <v>178</v>
@@ -2201,16 +2415,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>213</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Other food away from home</v>
+      <c r="C15" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="D15" t="s">
         <v>42</v>
@@ -2225,16 +2438,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>214</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Alcoholic beverages</v>
+      <c r="C16" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
@@ -2249,16 +2461,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>215</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Beer &amp; related drinks at home</v>
+      <c r="C17" s="1" t="s">
+        <v>491</v>
       </c>
       <c r="D17" t="s">
         <v>44</v>
@@ -2273,16 +2484,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Distilled spirits at home</v>
+      <c r="C18" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="D18" t="s">
         <v>45</v>
@@ -2297,16 +2507,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>217</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="C19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Wine at home</v>
+      <c r="C19" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="D19" t="s">
         <v>46</v>
@@ -2321,16 +2530,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>218</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="C20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Alcoholic beverages (away)</v>
+      <c r="C20" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="D20" t="s">
         <v>47</v>
@@ -2345,16 +2553,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>219</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="C21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">CPI - Nonalcoholic beverages </v>
+      <c r="C21" s="1" t="s">
+        <v>493</v>
       </c>
       <c r="D21" t="s">
         <v>48</v>
@@ -2369,16 +2576,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>220</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Carbonated drinks</v>
+      <c r="C22" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="D22" t="s">
         <v>49</v>
@@ -2393,16 +2599,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>221</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Frozen noncarbonated drinks</v>
+      <c r="C23" s="1" t="s">
+        <v>548</v>
       </c>
       <c r="D23" t="s">
         <v>179</v>
@@ -2417,16 +2622,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Nonfrozen noncarbonated drinks</v>
+      <c r="C24" s="1" t="s">
+        <v>494</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
@@ -2441,16 +2645,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Coffee</v>
+      <c r="C25" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="D25" t="s">
         <v>52</v>
@@ -2465,16 +2668,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>224</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="C26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Other beverages (e.g. tea)</v>
+      <c r="C26" s="1" t="s">
+        <v>495</v>
       </c>
       <c r="D26" t="s">
         <v>53</v>
@@ -2489,16 +2691,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>225</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="C27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Housing</v>
+      <c r="C27" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="D27" t="s">
         <v>54</v>
@@ -2513,16 +2714,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>226</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Shelter</v>
+      <c r="C28" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="D28" t="s">
         <v>55</v>
@@ -2537,16 +2737,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>227</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="C29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Rent of primary residence</v>
+      <c r="C29" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="D29" t="s">
         <v>56</v>
@@ -2561,16 +2760,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>228</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C30" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Lodging away from goods</v>
+      <c r="C30" s="1" t="s">
+        <v>496</v>
       </c>
       <c r="D30" t="s">
         <v>57</v>
@@ -2585,16 +2783,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>229</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="C31" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Owners' equivalent rent</v>
+      <c r="C31" s="1" t="s">
+        <v>497</v>
       </c>
       <c r="D31" t="s">
         <v>58</v>
@@ -2609,16 +2806,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="C32" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Tenants' &amp; household insurance</v>
+      <c r="C32" s="1" t="s">
+        <v>549</v>
       </c>
       <c r="D32" t="s">
         <v>180</v>
@@ -2633,16 +2829,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>231</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="C33" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Fuels &amp; utilities</v>
+      <c r="C33" s="1" t="s">
+        <v>498</v>
       </c>
       <c r="D33" t="s">
         <v>60</v>
@@ -2657,16 +2852,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>232</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="C34" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Fuel oil &amp; other fuels</v>
+      <c r="C34" s="1" t="s">
+        <v>499</v>
       </c>
       <c r="D34" t="s">
         <v>61</v>
@@ -2681,16 +2875,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>233</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C35" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Electricity</v>
+      <c r="C35" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="D35" t="s">
         <v>62</v>
@@ -2705,16 +2898,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>234</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Utility (piped) gas service</v>
+      <c r="C36" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="D36" t="s">
         <v>63</v>
@@ -2729,16 +2921,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>235</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="C37" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Water &amp; sewerage maint.</v>
+      <c r="C37" s="1" t="s">
+        <v>500</v>
       </c>
       <c r="D37" t="s">
         <v>64</v>
@@ -2753,16 +2944,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>236</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="C38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Garbage &amp; trash collection</v>
+      <c r="C38" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="D38" t="s">
         <v>65</v>
@@ -2777,16 +2967,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>237</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C39" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - HH furnishings &amp; operations</v>
+      <c r="C39" s="1" t="s">
+        <v>502</v>
       </c>
       <c r="D39" t="s">
         <v>66</v>
@@ -2801,16 +2990,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>238</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="C40" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Window &amp; floor coverings</v>
+      <c r="C40" s="1" t="s">
+        <v>503</v>
       </c>
       <c r="D40" t="s">
         <v>67</v>
@@ -2825,16 +3013,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>239</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="C41" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Furniture &amp; bedding</v>
+      <c r="C41" s="1" t="s">
+        <v>504</v>
       </c>
       <c r="D41" t="s">
         <v>68</v>
@@ -2849,16 +3036,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>240</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="C42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Appliances</v>
+      <c r="C42" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="D42" t="s">
         <v>69</v>
@@ -2873,16 +3059,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>241</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C43" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Tools &amp; outdoor equipment</v>
+      <c r="C43" s="1" t="s">
+        <v>505</v>
       </c>
       <c r="D43" t="s">
         <v>70</v>
@@ -2897,16 +3082,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>242</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="C44" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Housekeeping supplies</v>
+      <c r="C44" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="D44" t="s">
         <v>71</v>
@@ -2921,16 +3105,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>243</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Household operations</v>
+      <c r="C45" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="D45" t="s">
         <v>181</v>
@@ -2945,16 +3128,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>244</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="C46" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Other HH equipment &amp; furnishing</v>
+      <c r="C46" s="1" t="s">
+        <v>506</v>
       </c>
       <c r="D46" t="s">
         <v>73</v>
@@ -2969,16 +3151,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>245</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="C47" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Apparel</v>
+      <c r="C47" s="1" t="s">
+        <v>245</v>
       </c>
       <c r="D47" t="s">
         <v>74</v>
@@ -2993,16 +3174,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>246</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="C48" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Men's apparel</v>
+      <c r="C48" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="D48" t="s">
         <v>75</v>
@@ -3017,16 +3197,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>247</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Boys' apparel</v>
+      <c r="C49" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="D49" t="s">
         <v>76</v>
@@ -3041,16 +3220,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>248</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="C50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Men's suits &amp; outerwear</v>
+      <c r="C50" s="1" t="s">
+        <v>507</v>
       </c>
       <c r="D50" t="s">
         <v>77</v>
@@ -3065,16 +3243,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>249</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C51" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Men's underwear, pajama &amp; swim</v>
+      <c r="C51" s="1" t="s">
+        <v>508</v>
       </c>
       <c r="D51" t="s">
         <v>78</v>
@@ -3089,16 +3266,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>250</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="C52" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Men's shirts &amp; sweaters</v>
+      <c r="C52" s="1" t="s">
+        <v>509</v>
       </c>
       <c r="D52" t="s">
         <v>79</v>
@@ -3113,16 +3289,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="C53" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Men's pants &amp; shorts</v>
+      <c r="C53" s="1" t="s">
+        <v>510</v>
       </c>
       <c r="D53" t="s">
         <v>80</v>
@@ -3137,16 +3312,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>252</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="C54" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Women's &amp; girls' goods</v>
+      <c r="C54" s="1" t="s">
+        <v>511</v>
       </c>
       <c r="D54" t="s">
         <v>81</v>
@@ -3161,16 +3335,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>253</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C55" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Girls' apparel</v>
+      <c r="C55" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="D55" t="s">
         <v>82</v>
@@ -3185,16 +3358,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>254</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C56" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Women's outerwear</v>
+      <c r="C56" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="D56" t="s">
         <v>83</v>
@@ -3209,16 +3381,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>255</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="C57" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Women's dresses</v>
+      <c r="C57" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="D57" t="s">
         <v>84</v>
@@ -3233,16 +3404,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>256</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C58" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Women's suits &amp; separates</v>
+      <c r="C58" s="1" t="s">
+        <v>512</v>
       </c>
       <c r="D58" t="s">
         <v>85</v>
@@ -3257,16 +3427,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>257</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="C59" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Women's underwear, pajama &amp; swim</v>
+      <c r="C59" s="1" t="s">
+        <v>513</v>
       </c>
       <c r="D59" t="s">
         <v>86</v>
@@ -3281,16 +3450,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>258</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="C60" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Footwear</v>
+      <c r="C60" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="D60" t="s">
         <v>87</v>
@@ -3305,16 +3473,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>259</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="C61" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Men's footwear</v>
+      <c r="C61" s="1" t="s">
+        <v>259</v>
       </c>
       <c r="D61" t="s">
         <v>88</v>
@@ -3329,16 +3496,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="C62" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Boys' &amp; girls' footwear</v>
+      <c r="C62" s="1" t="s">
+        <v>514</v>
       </c>
       <c r="D62" t="s">
         <v>89</v>
@@ -3353,16 +3519,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>261</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C63" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Women's footwear</v>
+      <c r="C63" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="D63" t="s">
         <v>90</v>
@@ -3377,16 +3542,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>262</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="C64" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Infants' &amp; toddlers' apparel</v>
+      <c r="C64" s="1" t="s">
+        <v>515</v>
       </c>
       <c r="D64" t="s">
         <v>91</v>
@@ -3401,16 +3565,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>263</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C65" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Jewelry &amp; watches</v>
+      <c r="C65" s="1" t="s">
+        <v>516</v>
       </c>
       <c r="D65" t="s">
         <v>92</v>
@@ -3425,16 +3588,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>264</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C66" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CPI - Transportation</v>
+      <c r="C66" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="D66" t="s">
         <v>93</v>
@@ -3449,16 +3611,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>265</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C67" s="1" t="str">
-        <f t="shared" ref="C67:C130" si="1">_xlfn.CONCAT("CPI - ",B67)</f>
-        <v>CPI - Private transportation</v>
+      <c r="C67" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="D67" t="s">
         <v>94</v>
@@ -3473,16 +3634,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>266</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C68" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - New vehicles</v>
+      <c r="C68" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="D68" t="s">
         <v>95</v>
@@ -3497,16 +3657,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>267</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C69" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Used cars &amp; trucks</v>
+      <c r="C69" s="1" t="s">
+        <v>517</v>
       </c>
       <c r="D69" t="s">
         <v>96</v>
@@ -3521,16 +3680,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>268</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="C70" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Leased cars &amp; trucks</v>
+      <c r="C70" s="1" t="s">
+        <v>518</v>
       </c>
       <c r="D70" t="s">
         <v>97</v>
@@ -3545,16 +3703,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>269</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="C71" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Gasoline (all types)</v>
+      <c r="C71" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="D71" t="s">
         <v>98</v>
@@ -3569,16 +3726,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>270</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="C72" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Motor vehicle parts &amp; equipment</v>
+      <c r="C72" s="1" t="s">
+        <v>519</v>
       </c>
       <c r="D72" t="s">
         <v>99</v>
@@ -3593,16 +3749,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>271</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="C73" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Motor vehicle maint. &amp; repair</v>
+      <c r="C73" s="1" t="s">
+        <v>520</v>
       </c>
       <c r="D73" t="s">
         <v>100</v>
@@ -3617,16 +3772,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>272</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Motor vehicle fees</v>
+      <c r="C74" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D74" t="s">
         <v>182</v>
@@ -3641,16 +3795,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>273</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="C75" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Public transportation</v>
+      <c r="C75" s="1" t="s">
+        <v>273</v>
       </c>
       <c r="D75" t="s">
         <v>102</v>
@@ -3665,16 +3818,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>274</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="C76" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Airline fares</v>
+      <c r="C76" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="D76" t="s">
         <v>103</v>
@@ -3689,16 +3841,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>275</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="C77" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Other intercity transportation</v>
+      <c r="C77" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="D77" t="s">
         <v>104</v>
@@ -3713,16 +3864,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>276</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C78" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Intracity transportation</v>
+      <c r="C78" s="1" t="s">
+        <v>276</v>
       </c>
       <c r="D78" t="s">
         <v>183</v>
@@ -3737,16 +3887,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>277</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="C79" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Medical care</v>
+      <c r="C79" s="1" t="s">
+        <v>277</v>
       </c>
       <c r="D79" t="s">
         <v>106</v>
@@ -3761,16 +3910,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>278</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="C80" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Medical care commodities</v>
+      <c r="C80" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="D80" t="s">
         <v>107</v>
@@ -3785,16 +3933,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>279</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C81" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Prescription drugs</v>
+      <c r="C81" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="D81" t="s">
         <v>108</v>
@@ -3809,16 +3956,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>280</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C82" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Nonprescription drugs</v>
+      <c r="C82" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="D82" t="s">
         <v>184</v>
@@ -3833,16 +3979,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>281</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="C83" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Medical equipment &amp; supplies</v>
+      <c r="C83" s="1" t="s">
+        <v>550</v>
       </c>
       <c r="D83" t="s">
         <v>185</v>
@@ -3857,16 +4002,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>282</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C84" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Medical care services</v>
+      <c r="C84" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="D84" t="s">
         <v>111</v>
@@ -3881,16 +4025,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>283</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C85" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Physicians' services</v>
+      <c r="C85" s="1" t="s">
+        <v>283</v>
       </c>
       <c r="D85" t="s">
         <v>112</v>
@@ -3905,16 +4048,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>284</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="C86" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Dental services</v>
+      <c r="C86" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="D86" t="s">
         <v>113</v>
@@ -3929,16 +4071,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>285</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="C87" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Eyeglasses &amp; eye care</v>
+      <c r="C87" s="1" t="s">
+        <v>521</v>
       </c>
       <c r="D87" t="s">
         <v>114</v>
@@ -3953,16 +4094,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>286</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="C88" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Hospital services</v>
+      <c r="C88" s="1" t="s">
+        <v>286</v>
       </c>
       <c r="D88" t="s">
         <v>115</v>
@@ -3977,16 +4117,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>287</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="C89" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Nursing homes &amp; day services</v>
+      <c r="C89" s="1" t="s">
+        <v>522</v>
       </c>
       <c r="D89" t="s">
         <v>116</v>
@@ -4001,16 +4140,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>288</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C90" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Health insurance</v>
+      <c r="C90" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="D90" t="s">
         <v>186</v>
@@ -4025,16 +4163,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>289</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="C91" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Recreation</v>
+      <c r="C91" s="1" t="s">
+        <v>289</v>
       </c>
       <c r="D91" t="s">
         <v>118</v>
@@ -4049,16 +4186,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>290</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C92" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Video &amp; audio</v>
+      <c r="C92" s="1" t="s">
+        <v>523</v>
       </c>
       <c r="D92" t="s">
         <v>119</v>
@@ -4073,16 +4209,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>291</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C93" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Televisions</v>
+      <c r="C93" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="D93" t="s">
         <v>120</v>
@@ -4097,16 +4232,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>292</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="C94" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Cable &amp; satellite TV service</v>
+      <c r="C94" s="1" t="s">
+        <v>524</v>
       </c>
       <c r="D94" t="s">
         <v>121</v>
@@ -4121,16 +4255,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>293</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="C95" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Video discs &amp; other (e.g. rental)</v>
+      <c r="C95" s="1" t="s">
+        <v>551</v>
       </c>
       <c r="D95" t="s">
         <v>187</v>
@@ -4145,16 +4278,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>294</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="C96" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Other video equipment</v>
+      <c r="C96" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="D96" t="s">
         <v>123</v>
@@ -4169,16 +4301,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>295</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="C97" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Audio equipment</v>
+      <c r="C97" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="D97" t="s">
         <v>124</v>
@@ -4193,16 +4324,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>296</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="C98" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Recorded music &amp; subscriptions</v>
+      <c r="C98" s="1" t="s">
+        <v>552</v>
       </c>
       <c r="D98" t="s">
         <v>188</v>
@@ -4217,16 +4347,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>297</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C99" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Pets, pet products &amp; services</v>
+      <c r="C99" s="1" t="s">
+        <v>525</v>
       </c>
       <c r="D99" t="s">
         <v>126</v>
@@ -4241,16 +4370,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>298</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="C100" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Pets &amp; pet products</v>
+      <c r="C100" s="1" t="s">
+        <v>526</v>
       </c>
       <c r="D100" t="s">
         <v>127</v>
@@ -4265,16 +4393,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>299</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C101" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Pet services (e.g. veterinary)</v>
+      <c r="C101" s="1" t="s">
+        <v>527</v>
       </c>
       <c r="D101" t="s">
         <v>128</v>
@@ -4289,16 +4416,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>300</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="C102" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Sporting goods</v>
+      <c r="C102" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="D102" t="s">
         <v>129</v>
@@ -4313,16 +4439,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>301</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C103" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Sports vehicles like bicycles</v>
+      <c r="C103" s="1" t="s">
+        <v>528</v>
       </c>
       <c r="D103" t="s">
         <v>130</v>
@@ -4337,16 +4462,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>302</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C104" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Sports equipment</v>
+      <c r="C104" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="D104" t="s">
         <v>131</v>
@@ -4361,16 +4485,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>303</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="C105" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Photography</v>
+      <c r="C105" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="D105" t="s">
         <v>132</v>
@@ -4385,16 +4508,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>304</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="C106" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Photo equipment &amp; supplies</v>
+      <c r="C106" s="1" t="s">
+        <v>529</v>
       </c>
       <c r="D106" t="s">
         <v>133</v>
@@ -4409,16 +4531,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="C107" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Photographers &amp; photo processing</v>
+      <c r="C107" s="1" t="s">
+        <v>553</v>
       </c>
       <c r="D107" t="s">
         <v>189</v>
@@ -4433,16 +4554,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>306</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="C108" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Other recreational goods</v>
+      <c r="C108" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="D108" t="s">
         <v>135</v>
@@ -4457,16 +4577,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>307</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C109" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Toys</v>
+      <c r="C109" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="D109" t="s">
         <v>136</v>
@@ -4481,16 +4600,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>308</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="C110" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Sewing machines, fabric &amp; supplies</v>
+      <c r="C110" s="1" t="s">
+        <v>530</v>
       </c>
       <c r="D110" t="s">
         <v>137</v>
@@ -4505,16 +4623,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>309</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C111" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Music instruments &amp; accessories</v>
+      <c r="C111" s="1" t="s">
+        <v>531</v>
       </c>
       <c r="D111" t="s">
         <v>138</v>
@@ -4529,16 +4646,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>310</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C112" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Other recreational services</v>
+      <c r="C112" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="D112" t="s">
         <v>139</v>
@@ -4553,16 +4669,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>311</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="C113" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Club membership</v>
+      <c r="C113" s="1" t="s">
+        <v>533</v>
       </c>
       <c r="D113" t="s">
         <v>140</v>
@@ -4577,16 +4692,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>312</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C114" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Admissions</v>
+      <c r="C114" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="D114" t="s">
         <v>141</v>
@@ -4601,16 +4715,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>313</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C115" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Fees for lessons or instructions</v>
+      <c r="C115" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="D115" t="s">
         <v>142</v>
@@ -4625,16 +4738,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>314</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="C116" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Recreational reading materials</v>
+      <c r="C116" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="D116" t="s">
         <v>143</v>
@@ -4649,16 +4761,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>315</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C117" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Newspapers &amp; magazines</v>
+      <c r="C117" s="1" t="s">
+        <v>554</v>
       </c>
       <c r="D117" t="s">
         <v>190</v>
@@ -4673,16 +4784,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>316</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C118" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Recreational books</v>
+      <c r="C118" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="D118" t="s">
         <v>191</v>
@@ -4697,16 +4807,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>317</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="C119" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Education &amp; communication</v>
+      <c r="C119" s="1" t="s">
+        <v>534</v>
       </c>
       <c r="D119" t="s">
         <v>146</v>
@@ -4721,16 +4830,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>318</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C120" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Education</v>
+      <c r="C120" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="D120" t="s">
         <v>147</v>
@@ -4745,16 +4853,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>319</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="C121" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Educational books &amp; supplies</v>
+      <c r="C121" s="1" t="s">
+        <v>535</v>
       </c>
       <c r="D121" t="s">
         <v>148</v>
@@ -4769,16 +4876,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>320</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="C122" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - College tuition &amp; fees</v>
+      <c r="C122" s="1" t="s">
+        <v>536</v>
       </c>
       <c r="D122" t="s">
         <v>149</v>
@@ -4793,16 +4899,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>321</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C123" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Elementary &amp; H.S. tuition and fees</v>
+      <c r="C123" s="1" t="s">
+        <v>537</v>
       </c>
       <c r="D123" t="s">
         <v>150</v>
@@ -4817,16 +4922,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>322</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C124" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Day care &amp; preschool</v>
+      <c r="C124" s="1" t="s">
+        <v>538</v>
       </c>
       <c r="D124" t="s">
         <v>151</v>
@@ -4841,16 +4945,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>323</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="C125" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Tech. and businses school costs</v>
+      <c r="C125" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="D125" t="s">
         <v>152</v>
@@ -4865,16 +4968,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>324</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C126" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Postage &amp; delivery services</v>
+      <c r="C126" s="1" t="s">
+        <v>540</v>
       </c>
       <c r="D126" t="s">
         <v>153</v>
@@ -4889,16 +4991,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>325</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C127" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Postage</v>
+      <c r="C127" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="D127" t="s">
         <v>154</v>
@@ -4913,16 +5014,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>326</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C128" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Delivery services</v>
+      <c r="C128" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="D128" t="s">
         <v>155</v>
@@ -4937,16 +5037,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>327</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C129" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Info. &amp; info. Processing</v>
+      <c r="C129" s="1" t="s">
+        <v>555</v>
       </c>
       <c r="D129" t="s">
         <v>192</v>
@@ -4961,16 +5060,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>328</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C130" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CPI - Wireless telephone services</v>
+      <c r="C130" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="D130" t="s">
         <v>193</v>
@@ -4985,16 +5083,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>329</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C131" s="1" t="str">
-        <f t="shared" ref="C131:C147" si="2">_xlfn.CONCAT("CPI - ",B131)</f>
-        <v>CPI - Residential telephone services</v>
+      <c r="C131" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="D131" t="s">
         <v>194</v>
@@ -5009,16 +5106,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>330</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="C132" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Computers &amp; peripherals</v>
+      <c r="C132" s="1" t="s">
+        <v>541</v>
       </c>
       <c r="D132" t="s">
         <v>159</v>
@@ -5033,16 +5129,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>331</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C133" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Computer software &amp; accessories</v>
+      <c r="C133" s="1" t="s">
+        <v>556</v>
       </c>
       <c r="D133" t="s">
         <v>195</v>
@@ -5057,16 +5152,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>332</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="C134" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Internet services &amp; elec. providers</v>
+      <c r="C134" s="1" t="s">
+        <v>542</v>
       </c>
       <c r="D134" t="s">
         <v>161</v>
@@ -5081,16 +5175,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>333</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="C135" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Other goods and services</v>
+      <c r="C135" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="D135" t="s">
         <v>162</v>
@@ -5105,16 +5198,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>334</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C136" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Tobacco &amp; smoking products</v>
+      <c r="C136" s="1" t="s">
+        <v>543</v>
       </c>
       <c r="D136" t="s">
         <v>163</v>
@@ -5129,16 +5221,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>335</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C137" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Cigarettes</v>
+      <c r="C137" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="D137" t="s">
         <v>164</v>
@@ -5153,16 +5244,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>336</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="C138" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Non-cigarette tabacco products</v>
+      <c r="C138" s="1" t="s">
+        <v>557</v>
       </c>
       <c r="D138" t="s">
         <v>196</v>
@@ -5177,16 +5267,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>337</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="C139" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Personal care</v>
+      <c r="C139" s="1" t="s">
+        <v>337</v>
       </c>
       <c r="D139" t="s">
         <v>166</v>
@@ -5201,16 +5290,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>338</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C140" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Personal care products</v>
+      <c r="C140" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="D140" t="s">
         <v>197</v>
@@ -5225,16 +5313,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>339</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C141" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Personal care services</v>
+      <c r="C141" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="D141" t="s">
         <v>198</v>
@@ -5249,16 +5336,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>340</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="C142" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Misc. personal services</v>
+      <c r="C142" s="1" t="s">
+        <v>544</v>
       </c>
       <c r="D142" t="s">
         <v>169</v>
@@ -5273,16 +5359,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>341</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C143" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Legal services</v>
+      <c r="C143" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="D143" t="s">
         <v>170</v>
@@ -5297,16 +5382,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>342</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C144" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Funeral expenses</v>
+      <c r="C144" s="1" t="s">
+        <v>342</v>
       </c>
       <c r="D144" t="s">
         <v>171</v>
@@ -5321,16 +5405,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>343</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="C145" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Laundry &amp; dry cleaning services</v>
+      <c r="C145" s="1" t="s">
+        <v>545</v>
       </c>
       <c r="D145" t="s">
         <v>172</v>
@@ -5345,16 +5428,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>344</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="C146" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Other apparel services</v>
+      <c r="C146" s="1" t="s">
+        <v>558</v>
       </c>
       <c r="D146" t="s">
         <v>199</v>
@@ -5369,16 +5451,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>345</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="C147" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CPI - Financial services</v>
+      <c r="C147" s="1" t="s">
+        <v>345</v>
       </c>
       <c r="D147" t="s">
         <v>174</v>
@@ -5420,9 +5501,9 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -5445,7 +5526,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -5468,7 +5549,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>12</v>
       </c>
@@ -5491,7 +5572,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>21</v>
       </c>
@@ -5514,7 +5595,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>30</v>
       </c>
@@ -5537,7 +5618,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>43</v>
       </c>
@@ -5560,7 +5641,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>72</v>
       </c>
@@ -5583,7 +5664,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>76</v>
       </c>
@@ -5606,7 +5687,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>80</v>
       </c>
@@ -5629,7 +5710,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>81</v>
       </c>
@@ -5652,7 +5733,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>88</v>
       </c>
@@ -5675,7 +5756,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>93</v>
       </c>
@@ -5698,7 +5779,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>96</v>
       </c>
@@ -5721,7 +5802,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>105</v>
       </c>
@@ -5744,7 +5825,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>115</v>
       </c>
@@ -5767,7 +5848,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>116</v>
       </c>
@@ -5790,7 +5871,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>127</v>
       </c>
@@ -5813,7 +5894,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>128</v>
       </c>
@@ -5836,7 +5917,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>129</v>
       </c>
@@ -5859,7 +5940,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>131</v>
       </c>
@@ -5882,7 +5963,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>136</v>
       </c>
@@ -5905,7 +5986,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>138</v>
       </c>
@@ -5928,7 +6009,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>139</v>
       </c>
@@ -5951,7 +6032,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>144</v>
       </c>

</xml_diff>